<commit_message>
listo para mi uso
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\OneDrive\Documents\GitHub\Bot_Telegram_Disney\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C9968-F3BA-47B0-B411-3C689FAD72BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A6F535-584B-4428-AB61-6C997AEA0498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>UserID</t>
   </si>
   <si>
     <t>Emails</t>
+  </si>
+  <si>
+    <t>HJVKJ@GMAIL.COM</t>
   </si>
 </sst>
 </file>
@@ -393,13 +396,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -409,6 +415,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>55656862326</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>